<commit_message>
Revert "Merge branch 'master' of https://github.com/anrong/ACQuote"
This reverts commit 66a1ffca4b36671d9299abcd5fab2a9bc62cc849, reversing
changes made to 1cf40add579bce9528c816ff9422e08558c710b7.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="643">
   <si>
     <t xml:space="preserve">COLD WEATHER PACKAGE WITH BREAKER BOX AND HEATERS (CHOOSE 1 OR 2 PHASE) </t>
   </si>
@@ -1987,6 +1987,9 @@
   </si>
   <si>
     <t>Dep</t>
+  </si>
+  <si>
+    <t>Excludes</t>
   </si>
   <si>
     <t>Pump</t>
@@ -3684,11 +3687,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F485"/>
+  <dimension ref="A1:G485"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,7 +3701,7 @@
     <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>425</v>
       </c>
@@ -3715,10 +3718,13 @@
         <v>630</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>57554461</v>
       </c>
@@ -3732,7 +3738,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>54539457</v>
       </c>
@@ -3747,13 +3753,13 @@
         <v>57554461</v>
       </c>
       <c r="E3" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>57155541</v>
       </c>
@@ -3768,13 +3774,13 @@
         <v>57554461</v>
       </c>
       <c r="E4" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F4" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>57425811</v>
       </c>
@@ -3789,13 +3795,13 @@
         <v>57554461</v>
       </c>
       <c r="E5" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F5" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>57436164</v>
       </c>
@@ -3810,13 +3816,13 @@
         <v>57554461</v>
       </c>
       <c r="E6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F6" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>57557001</v>
       </c>
@@ -3831,13 +3837,13 @@
         <v>57554461</v>
       </c>
       <c r="E7" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F7" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>57594947</v>
       </c>
@@ -3852,13 +3858,13 @@
         <v>57554461</v>
       </c>
       <c r="E8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F8" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>57612020</v>
       </c>
@@ -3873,13 +3879,13 @@
         <v>57554461</v>
       </c>
       <c r="E9" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F9" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>57617896</v>
       </c>
@@ -3894,13 +3900,13 @@
         <v>57554461</v>
       </c>
       <c r="E10" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F10" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>57699654</v>
       </c>
@@ -3915,13 +3921,13 @@
         <v>57554461</v>
       </c>
       <c r="E11" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F11" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>57699712</v>
       </c>
@@ -3936,13 +3942,13 @@
         <v>57554461</v>
       </c>
       <c r="E12" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F12" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>57701179</v>
       </c>
@@ -3957,13 +3963,13 @@
         <v>57554461</v>
       </c>
       <c r="E13" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F13" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>57706004</v>
       </c>
@@ -3978,13 +3984,13 @@
         <v>57554461</v>
       </c>
       <c r="E14" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="F14" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>57724395</v>
       </c>
@@ -3999,13 +4005,13 @@
         <v>57554461</v>
       </c>
       <c r="E15" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F15" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>57726812</v>
       </c>
@@ -4017,6 +4023,9 @@
       </c>
       <c r="E16" t="s">
         <v>629</v>
+      </c>
+      <c r="F16" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4034,10 +4043,10 @@
         <v>57726812</v>
       </c>
       <c r="E17" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F17" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4055,10 +4064,10 @@
         <v>57726812</v>
       </c>
       <c r="E18" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F18" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4076,10 +4085,10 @@
         <v>57726812</v>
       </c>
       <c r="E19" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F19" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4097,10 +4106,10 @@
         <v>57726812</v>
       </c>
       <c r="E20" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F20" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4118,10 +4127,10 @@
         <v>57726812</v>
       </c>
       <c r="E21" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F21" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4139,10 +4148,10 @@
         <v>57726812</v>
       </c>
       <c r="E22" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F22" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4158,6 +4167,9 @@
       <c r="E23" t="s">
         <v>629</v>
       </c>
+      <c r="F23" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -4174,10 +4186,10 @@
         <v>57844599</v>
       </c>
       <c r="E24" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F24" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4195,10 +4207,10 @@
         <v>57844599</v>
       </c>
       <c r="E25" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F25" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4216,10 +4228,10 @@
         <v>57844599</v>
       </c>
       <c r="E26" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F26" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4237,10 +4249,10 @@
         <v>57844599</v>
       </c>
       <c r="E27" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="F27" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4258,10 +4270,10 @@
         <v>57844599</v>
       </c>
       <c r="E28" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="F28" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4279,10 +4291,10 @@
         <v>57844599</v>
       </c>
       <c r="E29" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="F29" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4300,10 +4312,10 @@
         <v>57844599</v>
       </c>
       <c r="E30" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F30" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4321,10 +4333,10 @@
         <v>57844599</v>
       </c>
       <c r="E31" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F31" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4342,10 +4354,10 @@
         <v>57844599</v>
       </c>
       <c r="E32" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="F32" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/anrong/ACQuote""
This reverts commit 48d99d5cc27073f0d9d8c5c71684a0401dd84bb8.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="642">
   <si>
     <t xml:space="preserve">COLD WEATHER PACKAGE WITH BREAKER BOX AND HEATERS (CHOOSE 1 OR 2 PHASE) </t>
   </si>
@@ -1987,9 +1987,6 @@
   </si>
   <si>
     <t>Dep</t>
-  </si>
-  <si>
-    <t>Excludes</t>
   </si>
   <si>
     <t>Pump</t>
@@ -3687,11 +3684,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G485"/>
+  <dimension ref="A1:F485"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3701,7 +3698,7 @@
     <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>425</v>
       </c>
@@ -3718,13 +3715,10 @@
         <v>630</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>57554461</v>
       </c>
@@ -3738,7 +3732,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>54539457</v>
       </c>
@@ -3753,13 +3747,13 @@
         <v>57554461</v>
       </c>
       <c r="E3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F3" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>57155541</v>
       </c>
@@ -3774,13 +3768,13 @@
         <v>57554461</v>
       </c>
       <c r="E4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F4" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>57425811</v>
       </c>
@@ -3795,13 +3789,13 @@
         <v>57554461</v>
       </c>
       <c r="E5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F5" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>57436164</v>
       </c>
@@ -3816,13 +3810,13 @@
         <v>57554461</v>
       </c>
       <c r="E6" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F6" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>57557001</v>
       </c>
@@ -3837,13 +3831,13 @@
         <v>57554461</v>
       </c>
       <c r="E7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F7" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>57594947</v>
       </c>
@@ -3858,13 +3852,13 @@
         <v>57554461</v>
       </c>
       <c r="E8" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F8" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>57612020</v>
       </c>
@@ -3879,13 +3873,13 @@
         <v>57554461</v>
       </c>
       <c r="E9" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F9" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>57617896</v>
       </c>
@@ -3900,13 +3894,13 @@
         <v>57554461</v>
       </c>
       <c r="E10" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F10" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>57699654</v>
       </c>
@@ -3921,13 +3915,13 @@
         <v>57554461</v>
       </c>
       <c r="E11" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F11" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>57699712</v>
       </c>
@@ -3942,13 +3936,13 @@
         <v>57554461</v>
       </c>
       <c r="E12" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F12" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>57701179</v>
       </c>
@@ -3963,13 +3957,13 @@
         <v>57554461</v>
       </c>
       <c r="E13" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F13" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>57706004</v>
       </c>
@@ -3984,13 +3978,13 @@
         <v>57554461</v>
       </c>
       <c r="E14" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F14" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>57724395</v>
       </c>
@@ -4005,13 +3999,13 @@
         <v>57554461</v>
       </c>
       <c r="E15" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F15" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>57726812</v>
       </c>
@@ -4023,9 +4017,6 @@
       </c>
       <c r="E16" t="s">
         <v>629</v>
-      </c>
-      <c r="F16" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4043,10 +4034,10 @@
         <v>57726812</v>
       </c>
       <c r="E17" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4064,10 +4055,10 @@
         <v>57726812</v>
       </c>
       <c r="E18" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F18" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4085,10 +4076,10 @@
         <v>57726812</v>
       </c>
       <c r="E19" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F19" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4106,10 +4097,10 @@
         <v>57726812</v>
       </c>
       <c r="E20" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F20" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4127,10 +4118,10 @@
         <v>57726812</v>
       </c>
       <c r="E21" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F21" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4148,10 +4139,10 @@
         <v>57726812</v>
       </c>
       <c r="E22" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F22" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4167,9 +4158,6 @@
       <c r="E23" t="s">
         <v>629</v>
       </c>
-      <c r="F23" t="s">
-        <v>636</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -4186,10 +4174,10 @@
         <v>57844599</v>
       </c>
       <c r="E24" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F24" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4207,10 +4195,10 @@
         <v>57844599</v>
       </c>
       <c r="E25" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F25" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4228,10 +4216,10 @@
         <v>57844599</v>
       </c>
       <c r="E26" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F26" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4249,10 +4237,10 @@
         <v>57844599</v>
       </c>
       <c r="E27" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F27" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4270,10 +4258,10 @@
         <v>57844599</v>
       </c>
       <c r="E28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F28" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4291,10 +4279,10 @@
         <v>57844599</v>
       </c>
       <c r="E29" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F29" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4312,10 +4300,10 @@
         <v>57844599</v>
       </c>
       <c r="E30" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F30" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4333,10 +4321,10 @@
         <v>57844599</v>
       </c>
       <c r="E31" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F31" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4354,10 +4342,10 @@
         <v>57844599</v>
       </c>
       <c r="E32" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F32" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>